<commit_message>
wip Building test cases
</commit_message>
<xml_diff>
--- a/virsion 1.xlsx
+++ b/virsion 1.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21165" windowHeight="9330" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21165" windowHeight="9330" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Version 1" sheetId="1" r:id="rId1"/>
     <sheet name="Version 2" sheetId="2" r:id="rId2"/>
+    <sheet name="TestCases" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="49">
   <si>
     <t>package test</t>
   </si>
@@ -173,12 +174,152 @@
     <t>/* A future is not given to you.
 It is something you must take for yourself</t>
   </si>
+  <si>
+    <t>Case#</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>package ru.iitdgroup.nir;
+import org.testng.annotations.Test;
+/**
+ * Some experiments with TestNG
+ *
+ *
+ * look at
+ * https://testng.org/doc/
+ * https://www.tutorialspoint.com/testng/testng_overview.htm
+ *
+ */
+public class ExampleTest {
+    @Test
+    public void testSimple(){</t>
+  </si>
+  <si>
+    <t>Expected behavior</t>
+  </si>
+  <si>
+    <t>keep all lines</t>
+  </si>
+  <si>
+    <t>package ru.iitdgroup.nir;
+import org.testng.annotations.Test;
+public class ExampleTest {
+       @Test
+    public void testSimple(){</t>
+  </si>
+  <si>
+    <t>package ru.iitdgroup.nir;
+import org.testng.annotations.Test;
+public class ExampleTest {
+ //    @Test
+    public void testSimple(){</t>
+  </si>
+  <si>
+    <t>remove javadoc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">package ru.iitdgroup.nir;
+import org.testng.annotations.Test;
+public class ExampleTest {
+       /*
+can u tall the difference between
+ multi comment and Javadoc
+*/
+/**
+*
+*
+*I suppose were about to find out now 
+*/
+    public void testSimple(){
+</t>
+  </si>
+  <si>
+    <t>package ru.iitdgroup.nir;
+import org.testng.annotations.Test;
+public class ExampleTest {
+/**The HelloWorld program implements an application that
+ * simply displays "Hello World
+*/
+{ 
+    // our program begins with a call to main()
+    // Prints "Hello, World
+    public static void main(String args[]) 
+    { 
+        System.out.println("Hello, World"); 
+    } 
+} 
+    public void testSimple(){</t>
+  </si>
+  <si>
+    <t>package ru.iitdgroup.nir;
+import org.testng.annotations.Test;
+public class ExampleTest {
+/*
+Sum of two numbers
+*/
+public class AddTwoNumbers {
+   public static void main(String[] args) {
+      int num1 = 5, num2 = 15, sum;
+      sum = num1 + num2;
+      System.out.println("Sum of these numbers: "+sum);
+   }
+}
+    public void testSimple(){</t>
+  </si>
+  <si>
+    <t>package ru.iitdgroup.nir;
+import org.testng.annotations.Test;
+public class ExampleTest {
+class Integers {
+  public static void main(String[] arguments) {
+    int c; //declaring a variable
+  /* Using a for loop to repeat instruction execution */
+    for (c = 1; c &lt;= 10; c++) {
+      System.out.println(c);
+    }
+  }
+}
+    public void testSimple(){</t>
+  </si>
+  <si>
+    <t>package ru.iitdgroup.nir;
+import org.testng.annotations.Test;
+public class ExampleTest {
+//test *1
+/*
+test 2
+*/
+    public void testSimple(){</t>
+  </si>
+  <si>
+    <t>package ru.iitdgroup.nir;
+import org.testng.annotations.Test;
+public class ExampleTest {
+//*
+ test 3
+*/
+ public static void main(String args[]) 
+    { 
+        System.out.println("Hello, World"); 
+    } 
+} 
+/*
+keep this line
+*/
+    public void testSimple(){</t>
+  </si>
+  <si>
+    <t>remove javadoc
+keep multi line</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -214,12 +355,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF808080"/>
-      <name val="Consolas"/>
-      <family val="3"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="0"/>
@@ -235,6 +370,36 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -283,23 +448,41 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
@@ -1286,7 +1469,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1471,8 +1654,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:J19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1511,7 +1694,7 @@
       </c>
     </row>
     <row r="4" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="8" t="s">
         <v>24</v>
       </c>
       <c r="E4" t="s">
@@ -1522,7 +1705,7 @@
       </c>
     </row>
     <row r="5" spans="3:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="4" t="s">
         <v>29</v>
       </c>
       <c r="E5" t="s">
@@ -1539,7 +1722,7 @@
       </c>
     </row>
     <row r="6" spans="3:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="4" t="s">
         <v>30</v>
       </c>
       <c r="E6" t="s">
@@ -1576,7 +1759,7 @@
       </c>
     </row>
     <row r="9" spans="3:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="4" t="s">
         <v>31</v>
       </c>
       <c r="E9" t="s">
@@ -1593,7 +1776,7 @@
       </c>
     </row>
     <row r="10" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="4" t="s">
         <v>3</v>
       </c>
       <c r="E10" t="s">
@@ -1607,15 +1790,15 @@
       </c>
     </row>
     <row r="11" spans="3:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="8"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="7"/>
     </row>
     <row r="12" spans="3:10" ht="120.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="4" t="s">
         <v>26</v>
       </c>
       <c r="E12" t="s">
@@ -1641,7 +1824,7 @@
       <c r="F13" t="s">
         <v>14</v>
       </c>
-      <c r="J13" s="7"/>
+      <c r="J13" s="6"/>
     </row>
     <row r="14" spans="3:10" x14ac:dyDescent="0.25">
       <c r="D14" s="1" t="s">
@@ -1661,7 +1844,7 @@
       </c>
     </row>
     <row r="15" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="4" t="s">
         <v>32</v>
       </c>
       <c r="E15" t="s">
@@ -1672,7 +1855,7 @@
       </c>
     </row>
     <row r="16" spans="3:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="4" t="s">
         <v>33</v>
       </c>
       <c r="E16" t="s">
@@ -1716,4 +1899,296 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C42"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="88.5" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="43" style="12" customWidth="1"/>
+    <col min="2" max="2" width="93" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" style="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="12">
+        <v>1</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="12">
+        <v>2</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="12">
+        <v>3</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="12">
+        <v>4</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="12">
+        <v>5</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="12">
+        <v>6</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="12">
+        <v>7</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="12">
+        <v>8</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="12">
+        <v>9</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="12">
+        <v>10</v>
+      </c>
+      <c r="B11" s="13"/>
+    </row>
+    <row r="12" spans="1:3" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="12">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="12">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="12">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="12">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="12">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="12">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="12">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="12">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="12">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="12">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="12">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="12">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="12">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="12">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="12">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="12">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="12">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="12">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="12">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="12">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="12">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="12">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="12">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="12">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="12">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="12">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="12">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="12">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="12">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="12">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Doing some testCases exercises
</commit_message>
<xml_diff>
--- a/virsion 1.xlsx
+++ b/virsion 1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21165" windowHeight="9330" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21165" windowHeight="9330" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Version 1" sheetId="1" r:id="rId1"/>
@@ -319,7 +319,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -373,11 +373,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Consolas"/>
-      <family val="3"/>
-    </font>
-    <font>
       <b/>
       <u/>
       <sz val="11"/>
@@ -401,6 +396,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="4">
@@ -451,7 +459,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -463,18 +471,15 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="2" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -482,6 +487,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1469,7 +1481,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1654,13 +1666,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:J19"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="6" width="22.140625" customWidth="1"/>
+    <col min="4" max="4" width="94.85546875" customWidth="1"/>
+    <col min="5" max="6" width="22.140625" customWidth="1"/>
     <col min="7" max="7" width="26.28515625" customWidth="1"/>
     <col min="8" max="8" width="16" customWidth="1"/>
   </cols>
@@ -1683,7 +1696,7 @@
       </c>
     </row>
     <row r="3" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="14" t="s">
         <v>25</v>
       </c>
       <c r="E3" t="s">
@@ -1694,7 +1707,7 @@
       </c>
     </row>
     <row r="4" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="15" t="s">
         <v>24</v>
       </c>
       <c r="E4" t="s">
@@ -1704,8 +1717,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="3:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="D5" s="4" t="s">
+    <row r="5" spans="3:10" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="D5" s="16" t="s">
         <v>29</v>
       </c>
       <c r="E5" t="s">
@@ -1721,8 +1734,8 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="3:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="D6" s="4" t="s">
+    <row r="6" spans="3:10" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="D6" s="16" t="s">
         <v>30</v>
       </c>
       <c r="E6" t="s">
@@ -1733,7 +1746,7 @@
       </c>
     </row>
     <row r="7" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="D7" s="1"/>
+      <c r="D7" s="14"/>
       <c r="E7" t="s">
         <v>8</v>
       </c>
@@ -1742,7 +1755,7 @@
       </c>
     </row>
     <row r="8" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="14" t="s">
         <v>3</v>
       </c>
       <c r="E8" t="s">
@@ -1758,8 +1771,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="3:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="D9" s="4" t="s">
+    <row r="9" spans="3:10" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="D9" s="16" t="s">
         <v>31</v>
       </c>
       <c r="E9" t="s">
@@ -1776,7 +1789,7 @@
       </c>
     </row>
     <row r="10" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="16" t="s">
         <v>3</v>
       </c>
       <c r="E10" t="s">
@@ -1905,285 +1918,285 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="88.5" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43" style="12" customWidth="1"/>
+    <col min="1" max="1" width="43" style="11" customWidth="1"/>
     <col min="2" max="2" width="93" customWidth="1"/>
-    <col min="3" max="3" width="17.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" style="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="12">
+      <c r="A2" s="11">
         <v>1</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="9" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="12">
+      <c r="A3" s="11">
         <v>2</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="9" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="12">
+      <c r="A4" s="11">
         <v>3</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="9" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="12">
+      <c r="A5" s="11">
         <v>4</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="9" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="12">
+      <c r="A6" s="11">
         <v>5</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="9" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="12">
+      <c r="A7" s="11">
         <v>6</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="9" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="12">
+      <c r="A8" s="11">
         <v>7</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="9" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="12">
+      <c r="A9" s="11">
         <v>8</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="9" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="12">
+      <c r="A10" s="11">
         <v>9</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="C10" s="13" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="12">
+      <c r="A11" s="11">
         <v>10</v>
       </c>
-      <c r="B11" s="13"/>
+      <c r="B11" s="12"/>
     </row>
     <row r="12" spans="1:3" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="12">
+      <c r="A12" s="11">
         <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="12">
+      <c r="A13" s="11">
         <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="12">
+      <c r="A14" s="11">
         <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="12">
+      <c r="A15" s="11">
         <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="12">
+      <c r="A16" s="11">
         <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="12">
+      <c r="A17" s="11">
         <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="12">
+      <c r="A18" s="11">
         <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:1" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="12">
+      <c r="A19" s="11">
         <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="12">
+      <c r="A20" s="11">
         <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:1" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="12">
+      <c r="A21" s="11">
         <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:1" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="12">
+      <c r="A22" s="11">
         <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:1" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="12">
+      <c r="A23" s="11">
         <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:1" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="12">
+      <c r="A24" s="11">
         <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:1" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="12">
+      <c r="A25" s="11">
         <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:1" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="12">
+      <c r="A26" s="11">
         <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:1" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="12">
+      <c r="A27" s="11">
         <v>26</v>
       </c>
     </row>
     <row r="28" spans="1:1" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="12">
+      <c r="A28" s="11">
         <v>27</v>
       </c>
     </row>
     <row r="29" spans="1:1" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="12">
+      <c r="A29" s="11">
         <v>28</v>
       </c>
     </row>
     <row r="30" spans="1:1" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="12">
+      <c r="A30" s="11">
         <v>29</v>
       </c>
     </row>
     <row r="31" spans="1:1" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="12">
+      <c r="A31" s="11">
         <v>30</v>
       </c>
     </row>
     <row r="32" spans="1:1" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="12">
+      <c r="A32" s="11">
         <v>31</v>
       </c>
     </row>
     <row r="33" spans="1:1" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="12">
+      <c r="A33" s="11">
         <v>32</v>
       </c>
     </row>
     <row r="34" spans="1:1" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="12">
+      <c r="A34" s="11">
         <v>33</v>
       </c>
     </row>
     <row r="35" spans="1:1" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="12">
+      <c r="A35" s="11">
         <v>34</v>
       </c>
     </row>
     <row r="36" spans="1:1" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="12">
+      <c r="A36" s="11">
         <v>35</v>
       </c>
     </row>
     <row r="37" spans="1:1" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="12">
+      <c r="A37" s="11">
         <v>36</v>
       </c>
     </row>
     <row r="38" spans="1:1" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="12">
+      <c r="A38" s="11">
         <v>37</v>
       </c>
     </row>
     <row r="39" spans="1:1" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="12">
+      <c r="A39" s="11">
         <v>38</v>
       </c>
     </row>
     <row r="40" spans="1:1" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="12">
+      <c r="A40" s="11">
         <v>39</v>
       </c>
     </row>
     <row r="41" spans="1:1" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="12">
+      <c r="A41" s="11">
         <v>40</v>
       </c>
     </row>
     <row r="42" spans="1:1" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="12">
+      <c r="A42" s="11">
         <v>41</v>
       </c>
     </row>

</xml_diff>